<commit_message>
Commit All Code still 05022023
Commit All Code still 05022023
</commit_message>
<xml_diff>
--- a/BRD/lead.xlsx
+++ b/BRD/lead.xlsx
@@ -4,59 +4,31 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="CAM Mapping" sheetId="4" r:id="rId3"/>
+    <sheet name="DocSignMapping" sheetId="5" r:id="rId4"/>
+    <sheet name="Final Approve" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Adress</t>
-  </si>
-  <si>
     <t>LeadID</t>
   </si>
   <si>
     <t>LeadNo</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>GuarantorID</t>
-  </si>
-  <si>
-    <t>tblLeadEntry</t>
-  </si>
-  <si>
-    <t>GuarantorType</t>
-  </si>
-  <si>
-    <t>"01/02"</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>tblLeadGuarantor</t>
-  </si>
-  <si>
-    <t>tblFOVerification</t>
-  </si>
-  <si>
-    <t>FOID</t>
-  </si>
-  <si>
     <t>StatusID</t>
   </si>
   <si>
@@ -316,22 +288,341 @@
   </si>
   <si>
     <t>ColletralSecurityType</t>
+  </si>
+  <si>
+    <t>CIBIL Verification</t>
+  </si>
+  <si>
+    <t>CIBILVerification,CibilDoc,CibilRemarks</t>
+  </si>
+  <si>
+    <t>Cash Flow &amp; basic CAM</t>
+  </si>
+  <si>
+    <t>CashFlowVerification,CashFlowDoc,CashFlowRemarks</t>
+  </si>
+  <si>
+    <t>FI STATUS</t>
+  </si>
+  <si>
+    <t>FIVerification,FIDoc,FIRemarks</t>
+  </si>
+  <si>
+    <t>TVR Status</t>
+  </si>
+  <si>
+    <t>TVRVerification,TVRDoc,TVRRemarks</t>
+  </si>
+  <si>
+    <t>Bank Statement Analysed</t>
+  </si>
+  <si>
+    <t>BankStmtVerification,BankStmtDoc,BankStmtRemarks</t>
+  </si>
+  <si>
+    <t>Income Assessment</t>
+  </si>
+  <si>
+    <t>IncomeStmtVerification,IncomeStmtDoc,IncomeStmtRemarks</t>
+  </si>
+  <si>
+    <t>Personal Discussion Sheet</t>
+  </si>
+  <si>
+    <t>PersonalDiscussVerification,PersonalDiscussDoc,PersonalDiscusssRemarks</t>
+  </si>
+  <si>
+    <t>Eligibility Sheet (FOIR)</t>
+  </si>
+  <si>
+    <t>Eligiblity,EligiblityDoc,EligiblityRemarks</t>
+  </si>
+  <si>
+    <t>Vehicle Valuation</t>
+  </si>
+  <si>
+    <t>ViechleValVerfication,ViechleDoc,ViechleRemarks</t>
+  </si>
+  <si>
+    <t>Occupancy</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Property Address</t>
+  </si>
+  <si>
+    <t>PropertyAddress</t>
+  </si>
+  <si>
+    <t>Property Size</t>
+  </si>
+  <si>
+    <t>PropertySize</t>
+  </si>
+  <si>
+    <t>Land Area</t>
+  </si>
+  <si>
+    <t>LandArea</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Value of Security</t>
+  </si>
+  <si>
+    <t>SecurityValue</t>
+  </si>
+  <si>
+    <t>Market Value</t>
+  </si>
+  <si>
+    <t>MarketValue</t>
+  </si>
+  <si>
+    <t>Land Value</t>
+  </si>
+  <si>
+    <t>LandValue</t>
+  </si>
+  <si>
+    <t>Construction Value</t>
+  </si>
+  <si>
+    <t>ConstrutionValue</t>
+  </si>
+  <si>
+    <t>Total Market value</t>
+  </si>
+  <si>
+    <t>TotalMarketValue</t>
+  </si>
+  <si>
+    <t>LTV</t>
+  </si>
+  <si>
+    <t>Relizable Value</t>
+  </si>
+  <si>
+    <t>RelizableValue</t>
+  </si>
+  <si>
+    <t>Property Title Documents</t>
+  </si>
+  <si>
+    <t>PropertyDocuments</t>
+  </si>
+  <si>
+    <t>Propery Chain</t>
+  </si>
+  <si>
+    <t>PropertyChain</t>
+  </si>
+  <si>
+    <t>Legal Opinion By</t>
+  </si>
+  <si>
+    <t>LegalOpinionBy</t>
+  </si>
+  <si>
+    <t>Legal Report Dated</t>
+  </si>
+  <si>
+    <t>LegalReportDate</t>
+  </si>
+  <si>
+    <t>Name of Valuer</t>
+  </si>
+  <si>
+    <t>ValuerName</t>
+  </si>
+  <si>
+    <t>Valuation as per valuer</t>
+  </si>
+  <si>
+    <t>Valuation</t>
+  </si>
+  <si>
+    <t>Valuation Report Date</t>
+  </si>
+  <si>
+    <t>ValueDate</t>
+  </si>
+  <si>
+    <t>Buisness name</t>
+  </si>
+  <si>
+    <t>BussinessName</t>
+  </si>
+  <si>
+    <t>Buisness Vintage</t>
+  </si>
+  <si>
+    <t>BussinessVinatage</t>
+  </si>
+  <si>
+    <t>Buisness Adress</t>
+  </si>
+  <si>
+    <t>BussinessAddress</t>
+  </si>
+  <si>
+    <t>Buisness Proof</t>
+  </si>
+  <si>
+    <t>BussinessProve</t>
+  </si>
+  <si>
+    <t>Collateral/Security Type</t>
+  </si>
+  <si>
+    <t>ColletralType</t>
+  </si>
+  <si>
+    <t>Credit team Remark</t>
+  </si>
+  <si>
+    <t>CreditRemarks</t>
+  </si>
+  <si>
+    <t>Negative Remarks</t>
+  </si>
+  <si>
+    <t>NegativeRemarks</t>
+  </si>
+  <si>
+    <t>Final CAM Preparataion</t>
+  </si>
+  <si>
+    <t>CAMGeneration,CAMDoc,CAMRemarks</t>
+  </si>
+  <si>
+    <t>Documents</t>
+  </si>
+  <si>
+    <t>Sanction Letter</t>
+  </si>
+  <si>
+    <t>SanctionLetter</t>
+  </si>
+  <si>
+    <t>Loan Agreement kit</t>
+  </si>
+  <si>
+    <t>LoanAgrmentKit</t>
+  </si>
+  <si>
+    <t>PDC</t>
+  </si>
+  <si>
+    <t>NACH</t>
+  </si>
+  <si>
+    <t>Disbursement Request letter</t>
+  </si>
+  <si>
+    <t>DisbursmentKit</t>
+  </si>
+  <si>
+    <t>Insurance With HP endorsed</t>
+  </si>
+  <si>
+    <t>InsuranceWithHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOC (Previous) If Financed </t>
+  </si>
+  <si>
+    <t>NOC</t>
+  </si>
+  <si>
+    <t>RTO SLIP</t>
+  </si>
+  <si>
+    <t>RTOSlip</t>
+  </si>
+  <si>
+    <t>Original Property Paper</t>
+  </si>
+  <si>
+    <t>OrignalPropertyPaper</t>
+  </si>
+  <si>
+    <t>Registered Mortgage Deed</t>
+  </si>
+  <si>
+    <t>RegisterdMortageDeed</t>
+  </si>
+  <si>
+    <t>Equitable Mortgage Deed</t>
+  </si>
+  <si>
+    <t>EquitableMortageDeed</t>
+  </si>
+  <si>
+    <t>Affidavit</t>
+  </si>
+  <si>
+    <t>Particular</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Loan Amount</t>
+  </si>
+  <si>
+    <t>Particulers</t>
+  </si>
+  <si>
+    <t>Processing Fees</t>
+  </si>
+  <si>
+    <t>Proccesfees</t>
+  </si>
+  <si>
+    <t>Advance EMI/Pre EMI</t>
+  </si>
+  <si>
+    <t>AdvanceEMI</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Net Disbursement Amount</t>
+  </si>
+  <si>
+    <t>NetDisbAmt</t>
+  </si>
+  <si>
+    <t>No of Tranches</t>
+  </si>
+  <si>
+    <t>TrnchsNo</t>
+  </si>
+  <si>
+    <t>CERSAI Charges</t>
+  </si>
+  <si>
+    <t>CersaiCharges</t>
+  </si>
+  <si>
+    <t>Stamping Charges</t>
+  </si>
+  <si>
+    <t>StamppingCharges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="7">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -350,6 +641,30 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -359,7 +674,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -395,18 +710,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,97 +1095,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -805,167 +1111,167 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
         <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="M2">
         <v>11</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="O2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="M3">
         <v>12</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M4">
         <v>13</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>2</v>
       </c>
       <c r="N6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O6" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="M7">
         <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="O7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1">
         <v>41619</v>
@@ -973,53 +1279,53 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="E16" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="5:5">
       <c r="E17" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="5:5">
       <c r="E18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1027,7 +1333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -1039,195 +1345,711 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A3" s="3" t="s">
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A4" s="3" t="s">
+      <c r="B13" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="3" t="s">
+      <c r="B14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A6" s="3" t="s">
+      <c r="B15" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A7" s="3" t="s">
+      <c r="B16" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="3" t="s">
+      <c r="B17" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="3" t="s">
+      <c r="B18" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="3" t="s">
+      <c r="B19" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A20" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A11" s="3" t="s">
+      <c r="B20" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A12" s="3" t="s">
+    </row>
+    <row r="22" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A22" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="A23" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A15" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A16" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A19" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A20" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A21" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A22" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="5" customFormat="1" ht="15.75" thickBot="1">
-      <c r="A23" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A1" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A10" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A11" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A12" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A13" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A14" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A16" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A17" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A19" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A20" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A21" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A22" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A23" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A24" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A25" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A26" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A27" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A28" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A29" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A30" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A31" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A32" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A33" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A35" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A36" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A7" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A8" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.5" thickBot="1">
+      <c r="A9" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45.75" thickBot="1">
+      <c r="A10" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60.75" thickBot="1">
+      <c r="A11" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="45.75" thickBot="1">
+      <c r="A12" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A13" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A1" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A3" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A4" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A5" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A6" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A7" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30.75" thickBot="1">
+      <c r="A8" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30.75" thickBot="1">
+      <c r="A9" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>